<commit_message>
grimoire fix, new method: magischer angriff
</commit_message>
<xml_diff>
--- a/data/held_josran_grimoire.xlsx
+++ b/data/held_josran_grimoire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaelm\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653A7E2D-C25A-42AE-A27C-BCCA08738736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6285AD-387F-4987-8B95-2EB1CDBB3DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Zauber</t>
   </si>
@@ -33,73 +33,61 @@
     <t>Eigenschaftsprobe</t>
   </si>
   <si>
-    <t>Dauer</t>
-  </si>
-  <si>
     <t>Kosten</t>
   </si>
   <si>
     <t>pro Stunde</t>
   </si>
   <si>
-    <t>Reichweite</t>
-  </si>
-  <si>
-    <t>Wirkdauer</t>
-  </si>
-  <si>
     <t>Bannbaladin</t>
   </si>
   <si>
     <t>MU/IN/CH</t>
   </si>
   <si>
-    <t>4 Aktionen</t>
-  </si>
-  <si>
     <t>8 AsP</t>
   </si>
   <si>
     <t>0 AsP</t>
   </si>
   <si>
-    <t>4 Schritt</t>
-  </si>
-  <si>
-    <t>15 Minuten</t>
-  </si>
-  <si>
     <t>Flim Flam</t>
   </si>
   <si>
     <t>MU/KL/CH</t>
   </si>
   <si>
-    <t>1 Aktion</t>
-  </si>
-  <si>
-    <t>2 Asp</t>
-  </si>
-  <si>
     <t>1 AsP</t>
   </si>
   <si>
-    <t>8 Schritt</t>
-  </si>
-  <si>
-    <t>aufrechthaltend</t>
-  </si>
-  <si>
     <t>Ignifaxius</t>
   </si>
   <si>
-    <t>2 Aktionen</t>
-  </si>
-  <si>
-    <t>16 Schritt</t>
-  </si>
-  <si>
-    <t>sofort</t>
+    <t>Schaden</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
+    <t>Zauberdauer</t>
+  </si>
+  <si>
+    <t>4 Aktion(en)</t>
+  </si>
+  <si>
+    <t>1 Aktion(en)</t>
+  </si>
+  <si>
+    <t>2 AsP</t>
+  </si>
+  <si>
+    <t>2 w6</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>2 Aktion(en)</t>
   </si>
 </sst>
 </file>
@@ -135,8 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -420,110 +411,111 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>